<commit_message>
Deploying to gh-pages from @ IDGRLP/Tumorkonferenzen-IG@e38de9f70783494dd6a3d2c1d975b63e268e7ea2 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-tnm-stage-group.xlsx
+++ b/StructureDefinition-tnm-stage-group.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$62</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="487">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-08T16:49:27+00:00</t>
+    <t>2024-04-08T16:58:24+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1367,6 +1367,76 @@
   </si>
   <si>
     <t xml:space="preserve">Reference(http://idg-rlp.de/fhir/tumorkonferenzen/StructureDefinition/TNMYSymbol)
+</t>
+  </si>
+  <si>
+    <t>Observation.hasMember:tnm-r-symbol</t>
+  </si>
+  <si>
+    <t>tnm-r-symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://idg-rlp.de/fhir/tumorkonferenzen/StructureDefinition/TNMRSymbol)
+</t>
+  </si>
+  <si>
+    <t>Observation.hasMember:tnm-a-symbol</t>
+  </si>
+  <si>
+    <t>tnm-a-symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://idg-rlp.de/fhir/tumorkonferenzen/StructureDefinition/TNMASymbol)
+</t>
+  </si>
+  <si>
+    <t>Observation.hasMember:tnm-m-symbol</t>
+  </si>
+  <si>
+    <t>tnm-m-symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://idg-rlp.de/fhir/tumorkonferenzen/StructureDefinition/TNMmSymbol)
+</t>
+  </si>
+  <si>
+    <t>Observation.hasMember:tnm-l-kategorie</t>
+  </si>
+  <si>
+    <t>tnm-l-kategorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://idg-rlp.de/fhir/tumorkonferenzen/StructureDefinition/TNMLKategorie)
+</t>
+  </si>
+  <si>
+    <t>Observation.hasMember:tnm-v-kategorie</t>
+  </si>
+  <si>
+    <t>tnm-v-kategorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://idg-rlp.de/fhir/tumorkonferenzen/StructureDefinition/TNMVKategorie)
+</t>
+  </si>
+  <si>
+    <t>Observation.hasMember:tnm-pn-kategorie</t>
+  </si>
+  <si>
+    <t>tnm-pn-kategorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://idg-rlp.de/fhir/tumorkonferenzen/StructureDefinition/TNMPnKategorie)
+</t>
+  </si>
+  <si>
+    <t>Observation.hasMember:tnm-s-kategorie</t>
+  </si>
+  <si>
+    <t>tnm-s-kategorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://idg-rlp.de/fhir/tumorkonferenzen/StructureDefinition/TNMSKategorie)
 </t>
   </si>
   <si>
@@ -1788,7 +1858,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AP55"/>
+  <dimension ref="A1:AP62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -7277,9 +7347,11 @@
         <v>431</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>431</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>402</v>
+      </c>
+      <c r="C46" t="s" s="2">
+        <v>432</v>
+      </c>
       <c r="D46" t="s" s="2">
         <v>80</v>
       </c>
@@ -7288,10 +7360,10 @@
         <v>78</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H46" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I46" t="s" s="2">
         <v>80</v>
@@ -7300,16 +7372,16 @@
         <v>92</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>433</v>
+        <v>404</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>434</v>
+        <v>405</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>435</v>
+        <v>406</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -7359,7 +7431,7 @@
         <v>80</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>431</v>
+        <v>402</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>78</v>
@@ -7383,7 +7455,7 @@
         <v>410</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>436</v>
+        <v>411</v>
       </c>
       <c r="AO46" t="s" s="2">
         <v>80</v>
@@ -7394,12 +7466,14 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>437</v>
-      </c>
-      <c r="C47" s="2"/>
+        <v>402</v>
+      </c>
+      <c r="C47" t="s" s="2">
+        <v>435</v>
+      </c>
       <c r="D47" t="s" s="2">
         <v>80</v>
       </c>
@@ -7408,10 +7482,10 @@
         <v>78</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I47" t="s" s="2">
         <v>80</v>
@@ -7420,20 +7494,18 @@
         <v>92</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>345</v>
+        <v>436</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>337</v>
+        <v>404</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>338</v>
+        <v>405</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>438</v>
-      </c>
-      <c r="O47" t="s" s="2">
-        <v>439</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
         <v>80</v>
       </c>
@@ -7481,7 +7553,7 @@
         <v>80</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>437</v>
+        <v>402</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>78</v>
@@ -7502,10 +7574,10 @@
         <v>80</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>440</v>
+        <v>410</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>441</v>
+        <v>411</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>80</v>
@@ -7516,12 +7588,14 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="C48" s="2"/>
+        <v>402</v>
+      </c>
+      <c r="C48" t="s" s="2">
+        <v>438</v>
+      </c>
       <c r="D48" t="s" s="2">
         <v>80</v>
       </c>
@@ -7533,24 +7607,26 @@
         <v>91</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I48" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>352</v>
+        <v>439</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>353</v>
+        <v>404</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="N48" s="2"/>
+        <v>405</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>406</v>
+      </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
         <v>80</v>
@@ -7599,19 +7675,19 @@
         <v>80</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>355</v>
+        <v>402</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>80</v>
@@ -7620,10 +7696,10 @@
         <v>80</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>80</v>
+        <v>410</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>356</v>
+        <v>411</v>
       </c>
       <c r="AO48" t="s" s="2">
         <v>80</v>
@@ -7634,42 +7710,44 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>443</v>
-      </c>
-      <c r="C49" s="2"/>
+        <v>402</v>
+      </c>
+      <c r="C49" t="s" s="2">
+        <v>441</v>
+      </c>
       <c r="D49" t="s" s="2">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>137</v>
+        <v>442</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>138</v>
+        <v>404</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>358</v>
+        <v>405</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>140</v>
+        <v>406</v>
       </c>
       <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
@@ -7719,7 +7797,7 @@
         <v>80</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>359</v>
+        <v>402</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>78</v>
@@ -7731,7 +7809,7 @@
         <v>80</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>80</v>
@@ -7740,10 +7818,10 @@
         <v>80</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>80</v>
+        <v>410</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>356</v>
+        <v>411</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>80</v>
@@ -7754,46 +7832,46 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="C50" t="s" s="2">
         <v>444</v>
       </c>
-      <c r="B50" t="s" s="2">
-        <v>444</v>
-      </c>
-      <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>361</v>
+        <v>80</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H50" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="J50" t="s" s="2">
         <v>92</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>137</v>
+        <v>445</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>362</v>
+        <v>404</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>363</v>
+        <v>405</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>140</v>
-      </c>
-      <c r="O50" t="s" s="2">
-        <v>146</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
         <v>80</v>
       </c>
@@ -7841,7 +7919,7 @@
         <v>80</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>364</v>
+        <v>402</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>78</v>
@@ -7853,7 +7931,7 @@
         <v>80</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>80</v>
@@ -7862,10 +7940,10 @@
         <v>80</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>80</v>
+        <v>410</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>134</v>
+        <v>411</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>80</v>
@@ -7876,24 +7954,26 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>445</v>
-      </c>
-      <c r="C51" s="2"/>
+        <v>402</v>
+      </c>
+      <c r="C51" t="s" s="2">
+        <v>447</v>
+      </c>
       <c r="D51" t="s" s="2">
         <v>80</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>91</v>
       </c>
       <c r="H51" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I51" t="s" s="2">
         <v>80</v>
@@ -7902,20 +7982,18 @@
         <v>92</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>189</v>
+        <v>448</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>446</v>
+        <v>404</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>447</v>
+        <v>405</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>448</v>
-      </c>
-      <c r="O51" t="s" s="2">
-        <v>203</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
         <v>80</v>
       </c>
@@ -7939,13 +8017,13 @@
         <v>80</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>311</v>
+        <v>80</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>449</v>
+        <v>80</v>
       </c>
       <c r="Z51" t="s" s="2">
-        <v>450</v>
+        <v>80</v>
       </c>
       <c r="AA51" t="s" s="2">
         <v>80</v>
@@ -7963,13 +8041,13 @@
         <v>80</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>445</v>
+        <v>402</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>80</v>
@@ -7981,16 +8059,16 @@
         <v>80</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>451</v>
+        <v>80</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>207</v>
+        <v>410</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>208</v>
+        <v>411</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>209</v>
+        <v>80</v>
       </c>
       <c r="AP51" t="s" s="2">
         <v>80</v>
@@ -7998,12 +8076,14 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>452</v>
-      </c>
-      <c r="C52" s="2"/>
+        <v>402</v>
+      </c>
+      <c r="C52" t="s" s="2">
+        <v>450</v>
+      </c>
       <c r="D52" t="s" s="2">
         <v>80</v>
       </c>
@@ -8015,7 +8095,7 @@
         <v>91</v>
       </c>
       <c r="H52" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I52" t="s" s="2">
         <v>80</v>
@@ -8024,20 +8104,18 @@
         <v>92</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>454</v>
+        <v>404</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>455</v>
+        <v>405</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>456</v>
-      </c>
-      <c r="O52" t="s" s="2">
-        <v>270</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
         <v>80</v>
       </c>
@@ -8085,13 +8163,13 @@
         <v>80</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>452</v>
+        <v>402</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>80</v>
@@ -8103,27 +8181,27 @@
         <v>80</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>457</v>
+        <v>80</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>274</v>
+        <v>410</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>275</v>
+        <v>411</v>
       </c>
       <c r="AO52" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP52" t="s" s="2">
-        <v>276</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -8134,7 +8212,7 @@
         <v>78</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H53" t="s" s="2">
         <v>80</v>
@@ -8143,23 +8221,21 @@
         <v>80</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>189</v>
+        <v>453</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>461</v>
-      </c>
-      <c r="O53" t="s" s="2">
-        <v>281</v>
-      </c>
+        <v>456</v>
+      </c>
+      <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
         <v>80</v>
       </c>
@@ -8183,13 +8259,13 @@
         <v>80</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>282</v>
+        <v>80</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>283</v>
+        <v>80</v>
       </c>
       <c r="Z53" t="s" s="2">
-        <v>284</v>
+        <v>80</v>
       </c>
       <c r="AA53" t="s" s="2">
         <v>80</v>
@@ -8207,16 +8283,16 @@
         <v>80</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH53" t="s" s="2">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>285</v>
+        <v>80</v>
       </c>
       <c r="AJ53" t="s" s="2">
         <v>103</v>
@@ -8228,10 +8304,10 @@
         <v>80</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>134</v>
+        <v>410</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>286</v>
+        <v>457</v>
       </c>
       <c r="AO53" t="s" s="2">
         <v>80</v>
@@ -8242,14 +8318,14 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
-        <v>288</v>
+        <v>80</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" t="s" s="2">
@@ -8265,22 +8341,22 @@
         <v>80</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>189</v>
+        <v>345</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>289</v>
+        <v>337</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>290</v>
+        <v>338</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>291</v>
+        <v>459</v>
       </c>
       <c r="O54" t="s" s="2">
-        <v>292</v>
+        <v>460</v>
       </c>
       <c r="P54" t="s" s="2">
         <v>80</v>
@@ -8305,13 +8381,13 @@
         <v>80</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>282</v>
+        <v>80</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>293</v>
+        <v>80</v>
       </c>
       <c r="Z54" t="s" s="2">
-        <v>294</v>
+        <v>80</v>
       </c>
       <c r="AA54" t="s" s="2">
         <v>80</v>
@@ -8329,7 +8405,7 @@
         <v>80</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>78</v>
@@ -8347,19 +8423,19 @@
         <v>80</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>295</v>
+        <v>80</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>296</v>
+        <v>461</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>297</v>
+        <v>462</v>
       </c>
       <c r="AO54" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AP54" t="s" s="2">
-        <v>298</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" hidden="true">
@@ -8378,7 +8454,7 @@
         <v>78</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>80</v>
@@ -8390,20 +8466,16 @@
         <v>80</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>81</v>
+        <v>352</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>464</v>
+        <v>353</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>465</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="O55" t="s" s="2">
-        <v>347</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
         <v>80</v>
       </c>
@@ -8451,41 +8523,893 @@
         <v>80</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>463</v>
+        <v>355</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH55" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AN55" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="AO55" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP55" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" hidden="true">
+      <c r="A56" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="B56" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G56" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="AI55" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AJ55" t="s" s="2">
+      <c r="H56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K56" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="N56" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="O56" s="2"/>
+      <c r="P56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q56" s="2"/>
+      <c r="R56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="AK56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AN56" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="AO56" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP56" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" hidden="true">
+      <c r="A57" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="B57" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G57" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I57" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="J57" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K57" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="M57" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="N57" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="O57" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="P57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q57" s="2"/>
+      <c r="R57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF57" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="AG57" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH57" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ57" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AN57" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="AO57" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP57" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" hidden="true">
+      <c r="A58" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="B58" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="G58" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="H58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J58" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K58" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="O58" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="P58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q58" s="2"/>
+      <c r="R58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X58" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="Y58" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="Z58" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="AA58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF58" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="AG58" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AH58" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ58" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="AK55" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AL55" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AM55" t="s" s="2">
+      <c r="AK58" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL58" t="s" s="2">
+        <v>472</v>
+      </c>
+      <c r="AM58" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="AN58" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="AO58" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="AP58" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" hidden="true">
+      <c r="A59" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="B59" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G59" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="H59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J59" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="K59" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="M59" t="s" s="2">
+        <v>476</v>
+      </c>
+      <c r="N59" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="O59" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="P59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q59" s="2"/>
+      <c r="R59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF59" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="AG59" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH59" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ59" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL59" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="AM59" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AN59" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="AO59" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP59" t="s" s="2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="60" hidden="true">
+      <c r="A60" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="B60" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G60" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="H60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K60" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="O60" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="P60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q60" s="2"/>
+      <c r="R60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X60" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="Y60" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="Z60" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AA60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF60" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="AG60" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH60" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="AI60" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AJ60" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM60" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="AN60" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="AO60" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP60" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" hidden="true">
+      <c r="A61" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="B61" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G61" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K61" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="L61" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="M61" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="N61" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="O61" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="P61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q61" s="2"/>
+      <c r="R61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X61" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="Y61" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="Z61" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AA61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF61" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="AG61" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH61" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL61" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="AM61" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="AN61" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AO61" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP61" t="s" s="2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="62" hidden="true">
+      <c r="A62" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="B62" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G62" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="N62" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="O62" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="P62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q62" s="2"/>
+      <c r="R62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF62" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="AG62" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH62" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ62" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM62" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="AN55" t="s" s="2">
+      <c r="AN62" t="s" s="2">
         <v>350</v>
       </c>
-      <c r="AO55" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AP55" t="s" s="2">
+      <c r="AO62" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AP62" t="s" s="2">
         <v>80</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP55">
+  <autoFilter ref="A1:AP62">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -8495,7 +9419,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI54">
+  <conditionalFormatting sqref="A2:AI61">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>